<commit_message>
Including 'Author' and 'UntaggedReportName'
git-svn-id: http://192.168.1.10/repos/toto@2721 b53939d4-f08c-4181-96d4-b201aa9c61c4
</commit_message>
<xml_diff>
--- a/Toto/trunk/web/WEB-INF/ReportMenu.xlsx
+++ b/Toto/trunk/web/WEB-INF/ReportMenu.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bill\projects\Toto\web\WEB-INF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFD0038-5F63-4102-90F4-3D7E5FA21015}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="Data">Sheet1!$A$5</definedName>
-    <definedName name="Title">Sheet1!$B$3</definedName>
+    <definedName name="Title">Sheet1!$D$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,15 +32,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Title of report</t>
   </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -466,33 +473,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:E3"/>
+  <dimension ref="B1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="53.28515625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="77" style="4" customWidth="1"/>
-    <col min="4" max="1026" width="11.5703125"/>
+    <col min="2" max="2" width="21.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="65.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="4" customWidth="1"/>
+    <col min="6" max="1028" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
-    <row r="3" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3"/>
+      <c r="E3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>